<commit_message>
que andas a fzr
</commit_message>
<xml_diff>
--- a/Trab3/Tabela secante 2.2.xlsx
+++ b/Trab3/Tabela secante 2.2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ammit\Desktop\ISEL\2223\LEIC\s2\AC\AC\Trab3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rccon\Documents\AC\Trab3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B270B65-C466-4EAE-A2FF-D2A8B297A15E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27E2C058-EBBA-4BD3-AE9B-D92E87ED7B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10245" yWindow="0" windowWidth="10245" windowHeight="10920" xr2:uid="{070A9D18-D015-4E30-8F7F-1FD43C1A297B}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{070A9D18-D015-4E30-8F7F-1FD43C1A297B}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -218,21 +218,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -548,56 +549,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FEB7A44-6D86-485B-AE1C-DF1FE5842785}">
-  <dimension ref="G1:N22"/>
+  <dimension ref="I3:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="113" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" customWidth="1"/>
+    <col min="9" max="9" width="13.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-    </row>
-    <row r="2" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-    </row>
-    <row r="3" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="5" t="s">
+    <row r="3" spans="9:14" x14ac:dyDescent="0.45">
+      <c r="I3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="5"/>
+    <row r="4" spans="9:14" x14ac:dyDescent="0.45">
+      <c r="I4" s="3"/>
       <c r="J4" s="1" t="s">
         <v>4</v>
       </c>
@@ -607,12 +588,10 @@
       <c r="L4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-    </row>
-    <row r="5" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+    </row>
+    <row r="5" spans="9:14" x14ac:dyDescent="0.45">
       <c r="I5" s="1" t="s">
         <v>7</v>
       </c>
@@ -632,9 +611,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
+    <row r="6" spans="9:14" x14ac:dyDescent="0.45">
       <c r="I6" s="1"/>
       <c r="J6" s="1">
         <v>0</v>
@@ -652,9 +629,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+    <row r="7" spans="9:14" x14ac:dyDescent="0.45">
       <c r="I7" s="1" t="s">
         <v>8</v>
       </c>
@@ -674,9 +649,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
+    <row r="8" spans="9:14" x14ac:dyDescent="0.45">
       <c r="I8" s="1"/>
       <c r="J8" s="1">
         <v>1</v>
@@ -694,9 +667,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+    <row r="9" spans="9:14" x14ac:dyDescent="0.45">
       <c r="I9" s="1" t="s">
         <v>9</v>
       </c>
@@ -716,9 +687,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+    <row r="10" spans="9:14" x14ac:dyDescent="0.45">
       <c r="I10" s="1"/>
       <c r="J10" s="1">
         <v>1</v>
@@ -736,9 +705,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+    <row r="11" spans="9:14" x14ac:dyDescent="0.45">
       <c r="I11" s="1" t="s">
         <v>10</v>
       </c>
@@ -758,9 +725,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+    <row r="12" spans="9:14" x14ac:dyDescent="0.45">
       <c r="I12" s="1"/>
       <c r="J12" s="1">
         <v>1</v>
@@ -771,16 +736,14 @@
       <c r="L12" s="1">
         <v>0</v>
       </c>
-      <c r="M12" s="6" t="s">
+      <c r="M12" s="2" t="s">
         <v>41</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="7:14" x14ac:dyDescent="0.25">
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
+    <row r="13" spans="9:14" x14ac:dyDescent="0.45">
       <c r="I13" s="1" t="s">
         <v>11</v>
       </c>
@@ -800,7 +763,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="9:14" x14ac:dyDescent="0.45">
       <c r="I14" s="1" t="s">
         <v>12</v>
       </c>
@@ -820,7 +783,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="9:14" x14ac:dyDescent="0.45">
       <c r="I15" s="1"/>
       <c r="J15" s="1">
         <v>0</v>
@@ -838,7 +801,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="7:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="9:14" x14ac:dyDescent="0.45">
       <c r="I16" s="1" t="s">
         <v>13</v>
       </c>
@@ -858,7 +821,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="9:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="9:14" x14ac:dyDescent="0.45">
       <c r="I17" s="1"/>
       <c r="J17" s="1">
         <v>1</v>
@@ -876,31 +839,47 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="L18" t="s">
+    <row r="18" spans="9:14" x14ac:dyDescent="0.45">
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+    </row>
+    <row r="19" spans="9:14" x14ac:dyDescent="0.45">
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+    </row>
+    <row r="20" spans="9:14" x14ac:dyDescent="0.45">
+      <c r="L20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="L19" t="s">
+    <row r="21" spans="9:14" x14ac:dyDescent="0.45">
+      <c r="L21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="L20" t="s">
+    <row r="22" spans="9:14" x14ac:dyDescent="0.45">
+      <c r="L22" t="s">
         <v>16</v>
       </c>
-      <c r="N20" t="s">
+      <c r="N22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="L21" t="s">
+    <row r="23" spans="9:14" x14ac:dyDescent="0.45">
+      <c r="L23" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="9:14" x14ac:dyDescent="0.25">
-      <c r="L22" t="s">
+    <row r="24" spans="9:14" x14ac:dyDescent="0.45">
+      <c r="L24" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>